<commit_message>
added screenshot, excel, extentreportlistener
</commit_message>
<xml_diff>
--- a/src/main/java/com/Finale_CRM/data/TestData.xlsx
+++ b/src/main/java/com/Finale_CRM/data/TestData.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="contacts" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>fname</t>
   </si>
   <si>
     <t>lname</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Tom</t>
@@ -57,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -394,39 +392,89 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>